<commit_message>
multiple tracking and multiple templates
</commit_message>
<xml_diff>
--- a/WFP.ICT.Web/Templates/Tracking2.xlsx
+++ b/WFP.ICT.Web/Templates/Tracking2.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\ADSDataDirect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NET_PROJECTS\ADSDataDirect\WFP.ICT.Web\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Total Opens</t>
   </si>
@@ -50,15 +50,6 @@
     <t xml:space="preserve">Quantity </t>
   </si>
   <si>
-    <t>https://goo.gl/6X7QVW</t>
-  </si>
-  <si>
-    <t>https://goo.gl/Qz000K</t>
-  </si>
-  <si>
-    <t>https://goo.gl/tnDQZ4</t>
-  </si>
-  <si>
     <t>Sent</t>
   </si>
   <si>
@@ -71,30 +62,6 @@
     <t>Unsub</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Forwards</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 48</t>
-    </r>
-  </si>
-  <si>
     <t>Total clicks</t>
   </si>
   <si>
@@ -138,6 +105,18 @@
   </si>
   <si>
     <t>Compaign Results</t>
+  </si>
+  <si>
+    <t>Order Number:</t>
+  </si>
+  <si>
+    <t>Campaign Name:</t>
+  </si>
+  <si>
+    <t>Forwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -316,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -354,41 +333,56 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -408,20 +402,8 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,71 +1036,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>57151</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>108345</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="12" name="Picture 11">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF992A76-0C7C-40F5-B057-18D8F8570A6A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="White_Label" spid="_x0000_s2051"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="38100" y="438151"/>
-              <a:ext cx="2070495" cy="1057274"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1455,19 +1372,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="4.28515625" customWidth="1"/>
@@ -1480,36 +1397,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="A1" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -1528,29 +1445,29 @@
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
       <c r="D4" s="12"/>
-      <c r="H4" s="40"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="30" t="s">
-        <v>6</v>
+      <c r="J4" s="32" t="s">
+        <v>3</v>
       </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="26">
+      <c r="L4" s="29">
         <v>100000</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="40"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="30"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="26"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="16">
@@ -1558,31 +1475,31 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="40"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="31" t="s">
-        <v>7</v>
+      <c r="J7" s="33" t="s">
+        <v>4</v>
       </c>
       <c r="K7" s="7"/>
-      <c r="L7" s="25">
+      <c r="L7" s="28">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="40"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="31"/>
+      <c r="J8" s="33"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="25"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
@@ -1592,39 +1509,39 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="29"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="32" t="s">
-        <v>8</v>
+      <c r="J10" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" s="28">
+      <c r="L10" s="31">
         <v>0.02</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="29"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="32"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="28"/>
+      <c r="L11" s="31"/>
     </row>
     <row r="12" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
@@ -1634,153 +1551,174 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="17"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="29"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="24" t="s">
-        <v>9</v>
+      <c r="J13" s="27" t="s">
+        <v>6</v>
       </c>
       <c r="K13" s="9"/>
-      <c r="L13" s="27">
+      <c r="L13" s="30">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="29"/>
+      <c r="A14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="24"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="22"/>
+    </row>
     <row r="17" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="21">
+      <c r="C19" s="35">
         <v>100000</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="34"/>
-      <c r="H19" s="23"/>
+      <c r="F19" s="39"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="34"/>
-      <c r="L19" s="23"/>
+      <c r="J19" s="39"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="34"/>
-      <c r="H20" s="23"/>
+      <c r="F20" s="39"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="34"/>
-      <c r="L20" s="23"/>
+      <c r="J20" s="39"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="35">
+      <c r="C22" s="40">
         <v>0.1</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="35">
         <v>10000</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="34"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="39"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="35">
+      <c r="C25" s="40">
         <v>0.02</v>
       </c>
-      <c r="D25" s="36"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="21">
+      <c r="F25" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="35">
         <v>2000</v>
       </c>
-      <c r="J25" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="38">
+      <c r="J25" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="43">
         <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="34"/>
-      <c r="H26" s="21"/>
-      <c r="J26" s="37"/>
-      <c r="L26" s="38"/>
+      <c r="F26" s="39"/>
+      <c r="H26" s="35"/>
+      <c r="J26" s="42"/>
+      <c r="L26" s="43"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="39"/>
+      <c r="C28" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="26"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="4"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="35">
+      <c r="C31" s="40">
         <v>0</v>
       </c>
-      <c r="D31" s="36"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="35">
+      <c r="F31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="40">
         <f>H31/H22</f>
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="34"/>
-      <c r="H32" s="23"/>
-      <c r="J32" s="42"/>
-      <c r="L32" s="35"/>
+      <c r="F32" s="39"/>
+      <c r="H32" s="25"/>
+      <c r="J32" s="44"/>
+      <c r="L32" s="40"/>
     </row>
     <row r="35" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A35" s="19" t="s">
@@ -1794,86 +1732,432 @@
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="20"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39">
-        <v>500</v>
-      </c>
+    </row>
+    <row r="36" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="23"/>
+      <c r="L52" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="23"/>
+      <c r="L54" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
+      <c r="L56" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L60" s="21"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L61" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A39:I39"/>
+  <mergeCells count="64">
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="A56:K56"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A44:K44"/>
     <mergeCell ref="L31:L32"/>
     <mergeCell ref="J31:J32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="H31:H32"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
     <mergeCell ref="A1:M2"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H19:H20"/>
@@ -1887,10 +2171,10 @@
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D23"/>
     <mergeCell ref="C25:D26"/>
-    <mergeCell ref="C28:D29"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="L19:L20"/>
+    <mergeCell ref="C28:D29"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="L4:L5"/>
@@ -1900,17 +2184,19 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C14:G15"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H13:H14"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>